<commit_message>
clean data to fix bug; now traceless vote matrix is returned
</commit_message>
<xml_diff>
--- a/data/season2_cleaned.xlsx
+++ b/data/season2_cleaned.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="week 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -209,18 +209,6 @@
     <t xml:space="preserve">Halcyon - Runaway (feat. Valentina Franco) [NCS Release]</t>
   </si>
   <si>
-    <t xml:space="preserve">Ron Pope - A drop in the ocean [with lyrics]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OC ReMix #2514: Pokémon Red Version 'Moondrops' [Mt. Moon Cave] by Sockpuppet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yosi Horikawa - Bubbles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Umphrey's McGee - In The Kitchen (Album Version)</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -248,6 +236,18 @@
       </rPr>
       <t xml:space="preserve">」音源（再現</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ron Pope - A drop in the ocean [with lyrics]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OC ReMix #2514: Pokémon Red Version 'Moondrops' [Mt. Moon Cave] by Sockpuppet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yosi Horikawa - Bubbles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umphrey's McGee - In The Kitchen (Album Version)</t>
   </si>
   <si>
     <t xml:space="preserve">ODESZA - Say My Name (feat. Zyra) - Lyric Video</t>
@@ -1047,23 +1047,23 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="C8 C6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,25 +1408,25 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="C8 C3"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.62244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.48469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,26 +1749,7 @@
       </c>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="0" t="n">
-        <f aca="false">SUM(D2:D9)</f>
-        <v>7</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <f aca="false">SUM(E2:E9)</f>
-        <v>7</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <f aca="false">SUM(F2:F9)</f>
-        <v>7</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">SUM(G2:G9)</f>
-        <v>42</v>
-      </c>
-    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1788,23 +1769,23 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="C8 C18"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,26 +2123,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M65536"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="C8 C6"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2312,169 +2293,169 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="16.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">3*D5+2*E5+F5</f>
-        <v>4</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <f aca="false">G5+IF(I5&gt;0,0,3)</f>
-        <v>4</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="n">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">3*D6+2*E6+F6</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">G6+IF(I6&gt;0,0,3)</f>
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">3*D7+2*E7+F7</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">G7+IF(I7&gt;0,0,3)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">3*D8+2*E8+F8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">G8+IF(I8&gt;0,0,3)</f>
-        <v>4</v>
-      </c>
-      <c r="I8" s="1"/>
+        <v>5</v>
+      </c>
       <c r="J8" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">3*D9+2*E9+F9</f>
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">G9+IF(I9&gt;0,0,3)</f>
+        <v>4</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2494,14 +2475,14 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="C8 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5663265306123"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2838,19 +2819,19 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="1" sqref="C8 D30"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.62244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.05102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3180,25 +3161,25 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="C8 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.62244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.60714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3542,26 +3523,26 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.62244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.48469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3883,7 +3864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3902,26 +3883,26 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="C8 C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.62244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.48469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4250,26 +4231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="0" t="n">
-        <f aca="false">SUM(D2:D9)</f>
-        <v>7</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <f aca="false">SUM(E2:E9)</f>
-        <v>7</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <f aca="false">SUM(F2:F9)</f>
-        <v>7</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">SUM(G2:G9)</f>
-        <v>42</v>
-      </c>
-    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4289,25 +4251,25 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="C8 D10"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.62244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.48469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>